<commit_message>
# Práctica 5 acabada (segunda de lenguajes)
</commit_message>
<xml_diff>
--- a/Practicas/Entregable 1/Tabla epsilon.xlsx
+++ b/Practicas/Entregable 1/Tabla epsilon.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFA87CC-289F-404F-9039-84D66866370E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20C428D-EDB5-41A8-A181-980A6736C34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1785" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="160">
   <si>
     <t>q0</t>
   </si>
@@ -543,6 +543,9 @@
   </si>
   <si>
     <t>Tabla DFA (Script)</t>
+  </si>
+  <si>
+    <t>DFA Segunda Parte</t>
   </si>
 </sst>
 </file>
@@ -694,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -710,6 +713,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -722,20 +732,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -743,44 +739,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -791,36 +750,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_1" connectionId="4" xr16:uid="{DF02CFA1-3555-4CD1-ADAA-0A454C51D23A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="7">
-    <queryTableFields count="6">
-      <queryTableField id="1" name="q" tableColumnId="1"/>
-      <queryTableField id="2" name="A" tableColumnId="2"/>
-      <queryTableField id="3" name="C" tableColumnId="3"/>
-      <queryTableField id="4" name="G" tableColumnId="4"/>
-      <queryTableField id="5" name="T" tableColumnId="5"/>
-      <queryTableField id="6" name="tipo_estado" tableColumnId="6"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{179FEE48-35F4-42BD-BD01-B1CBD59916F1}" name="tabla_con_dfa_minimizado" displayName="tabla_con_dfa_minimizado" ref="A1:F11" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F11" xr:uid="{179FEE48-35F4-42BD-BD01-B1CBD59916F1}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E377056E-9647-46EB-A45D-579F652D26FC}" uniqueName="1" name="q" queryTableFieldId="1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{2E626D52-41BA-4F3C-971B-16B8C765E66B}" uniqueName="2" name="A" queryTableFieldId="2" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{D5C240B7-BF7D-44F2-A1FF-EFF3F41EEDC2}" uniqueName="3" name="C" queryTableFieldId="3" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{A63E42CF-C5CD-45D3-AEC3-2A76D0DAE377}" uniqueName="4" name="G" queryTableFieldId="4" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{634DB72C-3C76-4F07-A011-6488936056EB}" uniqueName="5" name="T" queryTableFieldId="5" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{8D6478F9-828E-4666-A64E-C735C957D84A}" uniqueName="6" name="tipo_estado" queryTableFieldId="6"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1124,18 +1053,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC115"/>
+  <dimension ref="A1:AC117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T95" sqref="T95"/>
+    <sheetView tabSelected="1" topLeftCell="I104" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L121" sqref="L121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1155,31 +1081,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="L1" s="10" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="L1" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
     </row>
     <row r="2" spans="2:24" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="3" t="s">
@@ -1203,21 +1129,21 @@
       <c r="I2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="S2" s="9" t="s">
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="S2" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
     </row>
     <row r="3" spans="2:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
@@ -1315,19 +1241,19 @@
       <c r="S4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="T4" s="11" t="s">
+      <c r="T4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="U4" s="11" t="s">
+      <c r="U4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="11" t="s">
+      <c r="V4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="11" t="s">
+      <c r="W4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="12">
+      <c r="X4" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1374,19 +1300,19 @@
       <c r="S5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="T5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="U5" s="11" t="s">
+      <c r="U5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V5" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W5" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X5" s="12">
+      <c r="V5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X5" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1433,19 +1359,19 @@
       <c r="S6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="T6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="U6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X6" s="12">
+      <c r="U6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X6" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1492,19 +1418,19 @@
       <c r="S7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="T7" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U7" s="11" t="s">
+      <c r="T7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V7" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W7" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X7" s="12">
+      <c r="V7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X7" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1551,19 +1477,19 @@
       <c r="S8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="T8" s="11" t="s">
+      <c r="T8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="U8" s="11" t="s">
+      <c r="U8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V8" s="11" t="s">
+      <c r="V8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W8" s="11" t="s">
+      <c r="W8" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="X8" s="12">
+      <c r="X8" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1610,19 +1536,19 @@
       <c r="S9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T9" s="11" t="s">
+      <c r="T9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="U9" s="11" t="s">
+      <c r="U9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V9" s="11" t="s">
+      <c r="V9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W9" s="11" t="s">
+      <c r="W9" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="X9" s="12">
+      <c r="X9" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1669,19 +1595,19 @@
       <c r="S10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="T10" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U10" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V10" s="11" t="s">
+      <c r="T10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W10" s="11" t="s">
+      <c r="W10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="X10" s="12">
+      <c r="X10" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1728,19 +1654,19 @@
       <c r="S11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="T11" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U11" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V11" s="11" t="s">
+      <c r="T11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W11" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X11" s="12">
+      <c r="W11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X11" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1787,19 +1713,19 @@
       <c r="S12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="T12" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U12" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V12" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W12" s="11" t="s">
+      <c r="T12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="X12" s="12">
+      <c r="X12" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1846,19 +1772,19 @@
       <c r="S13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="T13" s="11" t="s">
+      <c r="T13" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="U13" s="11" t="s">
+      <c r="U13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V13" s="11" t="s">
+      <c r="V13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W13" s="11" t="s">
+      <c r="W13" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="X13" s="12">
+      <c r="X13" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1905,19 +1831,19 @@
       <c r="S14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="T14" s="11" t="s">
+      <c r="T14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="U14" s="11" t="s">
+      <c r="U14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V14" s="11" t="s">
+      <c r="V14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W14" s="11" t="s">
+      <c r="W14" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="X14" s="12">
+      <c r="X14" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1964,19 +1890,19 @@
       <c r="S15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="T15" s="11" t="s">
+      <c r="T15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="U15" s="11" t="s">
+      <c r="U15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V15" s="11" t="s">
+      <c r="V15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W15" s="11" t="s">
+      <c r="W15" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="X15" s="12">
+      <c r="X15" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2023,19 +1949,19 @@
       <c r="S16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="T16" s="11" t="s">
+      <c r="T16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="U16" s="11" t="s">
+      <c r="U16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V16" s="11" t="s">
+      <c r="V16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W16" s="11" t="s">
+      <c r="W16" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="X16" s="12">
+      <c r="X16" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2082,19 +2008,19 @@
       <c r="S17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T17" s="11" t="s">
+      <c r="T17" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="U17" s="11" t="s">
+      <c r="U17" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V17" s="11" t="s">
+      <c r="V17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W17" s="11" t="s">
+      <c r="W17" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="X17" s="12">
+      <c r="X17" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2133,7 +2059,7 @@
       <c r="N18" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="O18" s="11" t="s">
+      <c r="O18" s="7" t="s">
         <v>18</v>
       </c>
       <c r="P18" s="4" t="s">
@@ -2142,19 +2068,19 @@
       <c r="S18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="T18" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U18" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V18" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W18" s="11" t="s">
+      <c r="T18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="X18" s="12">
+      <c r="X18" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2203,19 +2129,19 @@
       <c r="S19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="T19" s="11" t="s">
+      <c r="T19" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="U19" s="11" t="s">
+      <c r="U19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V19" s="11" t="s">
+      <c r="V19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W19" s="11" t="s">
+      <c r="W19" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="X19" s="12">
+      <c r="X19" s="8">
         <v>-1</v>
       </c>
     </row>
@@ -2262,19 +2188,19 @@
       <c r="S20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T20" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U20" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V20" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W20" s="11" t="s">
+      <c r="T20" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U20" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V20" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="X20" s="12">
+      <c r="X20" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2321,19 +2247,19 @@
       <c r="S21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T21" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U21" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V21" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W21" s="11" t="s">
+      <c r="T21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="X21" s="12">
+      <c r="X21" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2380,19 +2306,19 @@
       <c r="S22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T22" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U22" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V22" s="11" t="s">
+      <c r="T22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="W22" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X22" s="12">
+      <c r="W22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X22" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2439,19 +2365,19 @@
       <c r="S23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="T23" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U23" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V23" s="11" t="s">
+      <c r="T23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="W23" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X23" s="12">
+      <c r="W23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X23" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2498,19 +2424,19 @@
       <c r="S24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="T24" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U24" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V24" s="11" t="s">
+      <c r="T24" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U24" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="W24" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X24" s="12">
+      <c r="W24" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X24" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2557,19 +2483,19 @@
       <c r="S25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="T25" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U25" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V25" s="11" t="s">
+      <c r="T25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V25" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="W25" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X25" s="12">
+      <c r="W25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X25" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2616,19 +2542,19 @@
       <c r="S26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="T26" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U26" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V26" s="11" t="s">
+      <c r="T26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="W26" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X26" s="12">
+      <c r="W26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X26" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2675,19 +2601,19 @@
       <c r="S27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T27" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U27" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V27" s="11" t="s">
+      <c r="T27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V27" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="W27" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X27" s="12">
+      <c r="W27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X27" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2734,19 +2660,19 @@
       <c r="S28" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T28" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U28" s="11" t="s">
+      <c r="T28" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U28" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="V28" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W28" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X28" s="12">
+      <c r="V28" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W28" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X28" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2793,19 +2719,19 @@
       <c r="S29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T29" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U29" s="11" t="s">
+      <c r="T29" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U29" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="V29" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W29" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X29" s="12">
+      <c r="V29" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W29" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X29" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2852,19 +2778,19 @@
       <c r="S30" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="T30" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U30" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V30" s="11" t="s">
+      <c r="T30" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U30" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V30" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="W30" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X30" s="12">
+      <c r="W30" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X30" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2911,19 +2837,19 @@
       <c r="S31" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="T31" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U31" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V31" s="11" t="s">
+      <c r="T31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V31" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="W31" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X31" s="12">
+      <c r="W31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X31" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2970,19 +2896,19 @@
       <c r="S32" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="T32" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U32" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V32" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W32" s="11" t="s">
+      <c r="T32" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U32" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V32" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W32" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="X32" s="12">
+      <c r="X32" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3029,19 +2955,19 @@
       <c r="S33" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="T33" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U33" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V33" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W33" s="11" t="s">
+      <c r="T33" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U33" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V33" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W33" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="X33" s="12">
+      <c r="X33" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3088,19 +3014,19 @@
       <c r="S34" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="T34" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U34" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V34" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W34" s="11" t="s">
+      <c r="T34" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U34" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V34" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W34" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="X34" s="12">
+      <c r="X34" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3147,19 +3073,19 @@
       <c r="S35" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="T35" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U35" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V35" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W35" s="11" t="s">
+      <c r="T35" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U35" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V35" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W35" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="X35" s="12">
+      <c r="X35" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3206,19 +3132,19 @@
       <c r="S36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="T36" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U36" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V36" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W36" s="11" t="s">
+      <c r="T36" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U36" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V36" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W36" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="X36" s="12">
+      <c r="X36" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3265,19 +3191,19 @@
       <c r="S37" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="T37" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U37" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V37" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W37" s="11" t="s">
+      <c r="T37" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U37" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V37" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W37" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="X37" s="12">
+      <c r="X37" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3326,19 +3252,19 @@
       <c r="S38" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T38" s="11" t="s">
+      <c r="T38" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="U38" s="11" t="s">
+      <c r="U38" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V38" s="11" t="s">
+      <c r="V38" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W38" s="11" t="s">
+      <c r="W38" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="X38" s="12">
+      <c r="X38" s="8">
         <v>1</v>
       </c>
     </row>
@@ -3387,19 +3313,19 @@
       <c r="S39" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="T39" s="11" t="s">
+      <c r="T39" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="U39" s="11" t="s">
+      <c r="U39" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V39" s="11" t="s">
+      <c r="V39" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W39" s="11" t="s">
+      <c r="W39" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="X39" s="12">
+      <c r="X39" s="8">
         <v>1</v>
       </c>
     </row>
@@ -3448,19 +3374,19 @@
       <c r="S40" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="T40" s="11" t="s">
+      <c r="T40" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="U40" s="11" t="s">
+      <c r="U40" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V40" s="11" t="s">
+      <c r="V40" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W40" s="11" t="s">
+      <c r="W40" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="X40" s="12">
+      <c r="X40" s="8">
         <v>1</v>
       </c>
     </row>
@@ -3507,19 +3433,19 @@
       <c r="S41" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="T41" s="11" t="s">
+      <c r="T41" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="U41" s="11" t="s">
+      <c r="U41" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V41" s="11" t="s">
+      <c r="V41" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W41" s="11" t="s">
+      <c r="W41" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="X41" s="12">
+      <c r="X41" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3566,19 +3492,19 @@
       <c r="S42" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="T42" s="11" t="s">
+      <c r="T42" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="U42" s="11" t="s">
+      <c r="U42" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V42" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W42" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X42" s="12">
+      <c r="V42" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W42" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X42" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3625,19 +3551,19 @@
       <c r="S43" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T43" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U43" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V43" s="11" t="s">
+      <c r="T43" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U43" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V43" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W43" s="11" t="s">
+      <c r="W43" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="X43" s="12">
+      <c r="X43" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3684,19 +3610,19 @@
       <c r="S44" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="T44" s="11" t="s">
+      <c r="T44" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="U44" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V44" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W44" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X44" s="12">
+      <c r="U44" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V44" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W44" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X44" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3743,19 +3669,19 @@
       <c r="S45" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="T45" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U45" s="11" t="s">
+      <c r="T45" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U45" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V45" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W45" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X45" s="12">
+      <c r="V45" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W45" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X45" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3802,19 +3728,19 @@
       <c r="S46" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="T46" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U46" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V46" s="11" t="s">
+      <c r="T46" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U46" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V46" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W46" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X46" s="12">
+      <c r="W46" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X46" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3861,19 +3787,19 @@
       <c r="S47" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="T47" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U47" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V47" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W47" s="11" t="s">
+      <c r="T47" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U47" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V47" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W47" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="X47" s="12">
+      <c r="X47" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3922,19 +3848,19 @@
       <c r="S48" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="T48" s="11" t="s">
+      <c r="T48" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="U48" s="11" t="s">
+      <c r="U48" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V48" s="11" t="s">
+      <c r="V48" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W48" s="11" t="s">
+      <c r="W48" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="X48" s="12">
+      <c r="X48" s="8">
         <v>1</v>
       </c>
     </row>
@@ -3983,19 +3909,19 @@
       <c r="S49" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="T49" s="11" t="s">
+      <c r="T49" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="U49" s="11" t="s">
+      <c r="U49" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V49" s="11" t="s">
+      <c r="V49" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W49" s="11" t="s">
+      <c r="W49" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="X49" s="12">
+      <c r="X49" s="8">
         <v>1</v>
       </c>
     </row>
@@ -4044,19 +3970,19 @@
       <c r="S50" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="T50" s="11" t="s">
+      <c r="T50" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="U50" s="11" t="s">
+      <c r="U50" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V50" s="11" t="s">
+      <c r="V50" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W50" s="11" t="s">
+      <c r="W50" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="X50" s="12">
+      <c r="X50" s="8">
         <v>1</v>
       </c>
     </row>
@@ -4105,19 +4031,19 @@
       <c r="S51" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="T51" s="11" t="s">
+      <c r="T51" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="U51" s="11" t="s">
+      <c r="U51" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V51" s="11" t="s">
+      <c r="V51" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W51" s="11" t="s">
+      <c r="W51" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="X51" s="12">
+      <c r="X51" s="8">
         <v>1</v>
       </c>
     </row>
@@ -4166,19 +4092,19 @@
       <c r="S52" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="T52" s="11" t="s">
+      <c r="T52" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="U52" s="11" t="s">
+      <c r="U52" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V52" s="11" t="s">
+      <c r="V52" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W52" s="11" t="s">
+      <c r="W52" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="X52" s="12">
+      <c r="X52" s="8">
         <v>1</v>
       </c>
     </row>
@@ -4227,19 +4153,19 @@
       <c r="S53" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="T53" s="11" t="s">
+      <c r="T53" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="U53" s="11" t="s">
+      <c r="U53" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V53" s="11" t="s">
+      <c r="V53" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W53" s="11" t="s">
+      <c r="W53" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="X53" s="12">
+      <c r="X53" s="8">
         <v>1</v>
       </c>
     </row>
@@ -4289,19 +4215,19 @@
       <c r="S54" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T54" s="11" t="s">
+      <c r="T54" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="U54" s="11" t="s">
+      <c r="U54" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V54" s="11" t="s">
+      <c r="V54" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W54" s="11" t="s">
+      <c r="W54" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="X54" s="12">
+      <c r="X54" s="8">
         <v>1</v>
       </c>
     </row>
@@ -4326,67 +4252,67 @@
       <c r="S55" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="T55" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U55" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="V55" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W55" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X55" s="12">
+      <c r="T55" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U55" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V55" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W55" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X55" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L59" s="10" t="s">
+      <c r="L59" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="M59" s="10"/>
-      <c r="N59" s="10"/>
-      <c r="O59" s="10"/>
-      <c r="P59" s="10"/>
-      <c r="Q59" s="10"/>
-      <c r="R59" s="10"/>
-      <c r="S59" s="10"/>
-      <c r="T59" s="10"/>
-      <c r="U59" s="10"/>
-      <c r="V59" s="10"/>
-      <c r="W59" s="10"/>
-      <c r="X59" s="10"/>
-      <c r="Y59" s="10"/>
-      <c r="Z59" s="10"/>
-      <c r="AA59" s="10"/>
-      <c r="AB59" s="10"/>
-      <c r="AC59" s="10"/>
+      <c r="M59" s="13"/>
+      <c r="N59" s="13"/>
+      <c r="O59" s="13"/>
+      <c r="P59" s="13"/>
+      <c r="Q59" s="13"/>
+      <c r="R59" s="13"/>
+      <c r="S59" s="13"/>
+      <c r="T59" s="13"/>
+      <c r="U59" s="13"/>
+      <c r="V59" s="13"/>
+      <c r="W59" s="13"/>
+      <c r="X59" s="13"/>
+      <c r="Y59" s="13"/>
+      <c r="Z59" s="13"/>
+      <c r="AA59" s="13"/>
+      <c r="AB59" s="13"/>
+      <c r="AC59" s="13"/>
     </row>
     <row r="60" spans="1:29" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L60" s="9" t="s">
+      <c r="L60" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="M60" s="9"/>
-      <c r="N60" s="9"/>
-      <c r="O60" s="9"/>
-      <c r="P60" s="9"/>
-      <c r="R60" s="9" t="s">
+      <c r="M60" s="12"/>
+      <c r="N60" s="12"/>
+      <c r="O60" s="12"/>
+      <c r="P60" s="12"/>
+      <c r="R60" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="S60" s="9"/>
-      <c r="T60" s="9"/>
-      <c r="U60" s="9"/>
-      <c r="V60" s="9"/>
-      <c r="X60" s="9" t="s">
+      <c r="S60" s="12"/>
+      <c r="T60" s="12"/>
+      <c r="U60" s="12"/>
+      <c r="V60" s="12"/>
+      <c r="X60" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="Y60" s="9"/>
-      <c r="Z60" s="9"/>
-      <c r="AA60" s="9"/>
-      <c r="AB60" s="9"/>
-      <c r="AC60" s="9"/>
+      <c r="Y60" s="12"/>
+      <c r="Z60" s="12"/>
+      <c r="AA60" s="12"/>
+      <c r="AB60" s="12"/>
+      <c r="AC60" s="12"/>
     </row>
     <row r="61" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="M61" s="3" t="s">
@@ -4451,35 +4377,35 @@
       <c r="R62" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="S62" s="11" t="s">
+      <c r="S62" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="T62" s="11" t="s">
+      <c r="T62" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U62" s="11" t="s">
+      <c r="U62" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="V62" s="11" t="s">
+      <c r="V62" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="W62" s="11"/>
+      <c r="W62" s="7"/>
       <c r="X62" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="Y62" s="11" t="s">
+      <c r="Y62" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Z62" s="11" t="s">
+      <c r="Z62" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AA62" s="11" t="s">
+      <c r="AA62" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AB62" s="11" t="s">
+      <c r="AB62" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AC62" s="12">
+      <c r="AC62" s="8">
         <v>-1</v>
       </c>
     </row>
@@ -4504,42 +4430,42 @@
       <c r="R63" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="S63" s="11" t="s">
+      <c r="S63" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="T63" s="11" t="s">
+      <c r="T63" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U63" s="11" t="s">
+      <c r="U63" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="V63" s="11" t="s">
+      <c r="V63" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="W63" s="11"/>
+      <c r="W63" s="7"/>
       <c r="X63" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Y63" s="11" t="s">
+      <c r="Y63" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Z63" s="11" t="s">
+      <c r="Z63" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AA63" s="11" t="s">
+      <c r="AA63" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AB63" s="11" t="s">
+      <c r="AB63" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AC63" s="12">
+      <c r="AC63" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E64" s="3"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
       <c r="L64" s="3" t="s">
@@ -4560,42 +4486,42 @@
       <c r="R64" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="S64" s="11" t="s">
+      <c r="S64" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="T64" s="11" t="s">
+      <c r="T64" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U64" s="11" t="s">
+      <c r="U64" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="V64" s="11" t="s">
+      <c r="V64" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="W64" s="11"/>
+      <c r="W64" s="7"/>
       <c r="X64" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Y64" s="11" t="s">
+      <c r="Y64" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Z64" s="11" t="s">
+      <c r="Z64" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AA64" s="11" t="s">
+      <c r="AA64" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AB64" s="11" t="s">
+      <c r="AB64" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AC64" s="12">
+      <c r="AC64" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E65" s="3"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
       <c r="L65" s="3" t="s">
@@ -4616,42 +4542,42 @@
       <c r="R65" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="S65" s="11" t="s">
+      <c r="S65" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="T65" s="11" t="s">
+      <c r="T65" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U65" s="11" t="s">
+      <c r="U65" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="V65" s="11" t="s">
+      <c r="V65" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="W65" s="11"/>
+      <c r="W65" s="7"/>
       <c r="X65" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Y65" s="11" t="s">
+      <c r="Y65" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Z65" s="11" t="s">
+      <c r="Z65" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AA65" s="11" t="s">
+      <c r="AA65" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AB65" s="11" t="s">
+      <c r="AB65" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AC65" s="12">
+      <c r="AC65" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E66" s="3"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
       <c r="L66" s="3" t="s">
@@ -4672,42 +4598,42 @@
       <c r="R66" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="S66" s="11" t="s">
+      <c r="S66" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="T66" s="11" t="s">
+      <c r="T66" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U66" s="11" t="s">
+      <c r="U66" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V66" s="11" t="s">
+      <c r="V66" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="W66" s="11"/>
+      <c r="W66" s="7"/>
       <c r="X66" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Y66" s="11" t="s">
+      <c r="Y66" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Z66" s="11" t="s">
+      <c r="Z66" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AA66" s="11" t="s">
+      <c r="AA66" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AB66" s="11" t="s">
+      <c r="AB66" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AC66" s="12">
+      <c r="AC66" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E67" s="3"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
       <c r="L67" s="3" t="s">
@@ -4728,42 +4654,42 @@
       <c r="R67" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S67" s="11" t="s">
+      <c r="S67" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="T67" s="11" t="s">
+      <c r="T67" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U67" s="11" t="s">
+      <c r="U67" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="V67" s="11" t="s">
+      <c r="V67" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="W67" s="11"/>
+      <c r="W67" s="7"/>
       <c r="X67" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Y67" s="11" t="s">
+      <c r="Y67" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Z67" s="11" t="s">
+      <c r="Z67" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AA67" s="11" t="s">
+      <c r="AA67" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AB67" s="11" t="s">
+      <c r="AB67" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AC67" s="12">
+      <c r="AC67" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E68" s="3"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="L68" s="3" t="s">
@@ -4784,42 +4710,42 @@
       <c r="R68" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="S68" s="11" t="s">
+      <c r="S68" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="T68" s="11" t="s">
+      <c r="T68" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U68" s="11" t="s">
+      <c r="U68" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="V68" s="11" t="s">
+      <c r="V68" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="W68" s="11"/>
+      <c r="W68" s="7"/>
       <c r="X68" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="Y68" s="11" t="s">
+      <c r="Y68" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Z68" s="11" t="s">
+      <c r="Z68" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AA68" s="11" t="s">
+      <c r="AA68" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AB68" s="11" t="s">
+      <c r="AB68" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AC68" s="12">
+      <c r="AC68" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E69" s="3"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
       <c r="L69" s="3" t="s">
@@ -4840,42 +4766,42 @@
       <c r="R69" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="S69" s="11" t="s">
+      <c r="S69" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="T69" s="11" t="s">
+      <c r="T69" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="U69" s="11" t="s">
+      <c r="U69" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="V69" s="11" t="s">
+      <c r="V69" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="W69" s="11"/>
+      <c r="W69" s="7"/>
       <c r="X69" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Y69" s="11" t="s">
+      <c r="Y69" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Z69" s="11" t="s">
+      <c r="Z69" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AA69" s="11" t="s">
+      <c r="AA69" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AB69" s="11" t="s">
+      <c r="AB69" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AC69" s="12">
+      <c r="AC69" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E70" s="3"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="L70" s="3" t="s">
@@ -4896,42 +4822,42 @@
       <c r="R70" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="S70" s="11" t="s">
+      <c r="S70" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="T70" s="11" t="s">
+      <c r="T70" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U70" s="11" t="s">
+      <c r="U70" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="V70" s="11" t="s">
+      <c r="V70" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="W70" s="11"/>
+      <c r="W70" s="7"/>
       <c r="X70" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Y70" s="11" t="s">
+      <c r="Y70" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Z70" s="11" t="s">
+      <c r="Z70" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AA70" s="11" t="s">
+      <c r="AA70" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="AB70" s="11" t="s">
+      <c r="AB70" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AC70" s="12">
+      <c r="AC70" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E71" s="3"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
       <c r="L71" s="3" t="s">
@@ -4952,42 +4878,42 @@
       <c r="R71" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="S71" s="11" t="s">
+      <c r="S71" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="T71" s="11" t="s">
+      <c r="T71" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U71" s="11" t="s">
+      <c r="U71" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="V71" s="11" t="s">
+      <c r="V71" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="W71" s="11"/>
+      <c r="W71" s="7"/>
       <c r="X71" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Y71" s="11" t="s">
+      <c r="Y71" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Z71" s="11" t="s">
+      <c r="Z71" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AA71" s="11" t="s">
+      <c r="AA71" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AB71" s="11" t="s">
+      <c r="AB71" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="AC71" s="12">
+      <c r="AC71" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E72" s="3"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
       <c r="L72" s="3" t="s">
@@ -5008,42 +4934,42 @@
       <c r="R72" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="S72" s="11" t="s">
+      <c r="S72" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="T72" s="11" t="s">
+      <c r="T72" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U72" s="11" t="s">
+      <c r="U72" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V72" s="11" t="s">
+      <c r="V72" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="W72" s="11"/>
+      <c r="W72" s="7"/>
       <c r="X72" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Y72" s="11" t="s">
+      <c r="Y72" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Z72" s="11" t="s">
+      <c r="Z72" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AA72" s="11" t="s">
+      <c r="AA72" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AB72" s="11" t="s">
+      <c r="AB72" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="AC72" s="12">
+      <c r="AC72" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E73" s="3"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
       <c r="L73" s="3" t="s">
@@ -5064,42 +4990,42 @@
       <c r="R73" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="S73" s="11" t="s">
+      <c r="S73" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="T73" s="11" t="s">
+      <c r="T73" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U73" s="11" t="s">
+      <c r="U73" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V73" s="11" t="s">
+      <c r="V73" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="W73" s="11"/>
+      <c r="W73" s="7"/>
       <c r="X73" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Y73" s="11" t="s">
+      <c r="Y73" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Z73" s="11" t="s">
+      <c r="Z73" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AA73" s="11" t="s">
+      <c r="AA73" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AB73" s="11" t="s">
+      <c r="AB73" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AC73" s="12">
+      <c r="AC73" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E74" s="3"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
       <c r="K74" s="6"/>
@@ -5121,42 +5047,42 @@
       <c r="R74" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="S74" s="11" t="s">
+      <c r="S74" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T74" s="11" t="s">
+      <c r="T74" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U74" s="11" t="s">
+      <c r="U74" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V74" s="11" t="s">
+      <c r="V74" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="W74" s="11"/>
+      <c r="W74" s="7"/>
       <c r="X74" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Y74" s="11" t="s">
+      <c r="Y74" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z74" s="11" t="s">
+      <c r="Z74" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AA74" s="11" t="s">
+      <c r="AA74" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AB74" s="11" t="s">
+      <c r="AB74" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AC74" s="12">
+      <c r="AC74" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E75" s="3"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
       <c r="K75" s="6"/>
@@ -5169,7 +5095,7 @@
       <c r="N75" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="O75" s="11" t="s">
+      <c r="O75" s="7" t="s">
         <v>147</v>
       </c>
       <c r="P75" s="4" t="s">
@@ -5178,42 +5104,42 @@
       <c r="R75" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="S75" s="11" t="s">
+      <c r="S75" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T75" s="11" t="s">
+      <c r="T75" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U75" s="11" t="s">
+      <c r="U75" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="V75" s="11" t="s">
+      <c r="V75" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="W75" s="11"/>
+      <c r="W75" s="7"/>
       <c r="X75" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Y75" s="11" t="s">
+      <c r="Y75" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z75" s="11" t="s">
+      <c r="Z75" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AA75" s="11" t="s">
+      <c r="AA75" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AB75" s="11" t="s">
+      <c r="AB75" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AC75" s="12">
+      <c r="AC75" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E76" s="3"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
       <c r="K76" s="6"/>
@@ -5235,42 +5161,42 @@
       <c r="R76" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S76" s="11" t="s">
+      <c r="S76" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T76" s="11" t="s">
+      <c r="T76" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U76" s="11" t="s">
+      <c r="U76" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="V76" s="11" t="s">
+      <c r="V76" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="W76" s="11"/>
+      <c r="W76" s="7"/>
       <c r="X76" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Y76" s="11" t="s">
+      <c r="Y76" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z76" s="11" t="s">
+      <c r="Z76" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AA76" s="11" t="s">
+      <c r="AA76" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AB76" s="11" t="s">
+      <c r="AB76" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AC76" s="12">
+      <c r="AC76" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E77" s="3"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
       <c r="K77" s="6"/>
@@ -5292,42 +5218,42 @@
       <c r="R77" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="S77" s="11" t="s">
+      <c r="S77" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T77" s="11" t="s">
+      <c r="T77" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U77" s="11" t="s">
+      <c r="U77" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="V77" s="11" t="s">
+      <c r="V77" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="W77" s="11"/>
+      <c r="W77" s="7"/>
       <c r="X77" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Y77" s="11" t="s">
+      <c r="Y77" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z77" s="11" t="s">
+      <c r="Z77" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AA77" s="11" t="s">
+      <c r="AA77" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="AB77" s="11" t="s">
+      <c r="AB77" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AC77" s="12">
+      <c r="AC77" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E78" s="3"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
       <c r="K78" s="6"/>
@@ -5349,42 +5275,42 @@
       <c r="R78" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S78" s="11" t="s">
+      <c r="S78" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T78" s="11" t="s">
+      <c r="T78" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U78" s="11" t="s">
+      <c r="U78" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V78" s="11" t="s">
+      <c r="V78" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="W78" s="11"/>
+      <c r="W78" s="7"/>
       <c r="X78" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Y78" s="11" t="s">
+      <c r="Y78" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z78" s="11" t="s">
+      <c r="Z78" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AA78" s="11" t="s">
+      <c r="AA78" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AB78" s="11" t="s">
+      <c r="AB78" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AC78" s="12">
+      <c r="AC78" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E79" s="3"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
       <c r="K79" s="6"/>
@@ -5406,42 +5332,42 @@
       <c r="R79" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S79" s="11" t="s">
+      <c r="S79" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T79" s="11" t="s">
+      <c r="T79" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U79" s="11" t="s">
+      <c r="U79" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="V79" s="11" t="s">
+      <c r="V79" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="W79" s="11"/>
+      <c r="W79" s="7"/>
       <c r="X79" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Y79" s="11" t="s">
+      <c r="Y79" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z79" s="11" t="s">
+      <c r="Z79" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AA79" s="11" t="s">
+      <c r="AA79" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AB79" s="11" t="s">
+      <c r="AB79" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AC79" s="12">
+      <c r="AC79" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E80" s="3"/>
-      <c r="F80" s="11"/>
-      <c r="G80" s="11"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
       <c r="K80" s="6"/>
@@ -5463,42 +5389,42 @@
       <c r="R80" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S80" s="11" t="s">
+      <c r="S80" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T80" s="11" t="s">
+      <c r="T80" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U80" s="11" t="s">
+      <c r="U80" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="V80" s="11" t="s">
+      <c r="V80" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="W80" s="11"/>
+      <c r="W80" s="7"/>
       <c r="X80" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Y80" s="11" t="s">
+      <c r="Y80" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z80" s="11" t="s">
+      <c r="Z80" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AA80" s="11" t="s">
+      <c r="AA80" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="AB80" s="11" t="s">
+      <c r="AB80" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AC80" s="12">
+      <c r="AC80" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E81" s="3"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="11"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
       <c r="K81" s="6"/>
@@ -5520,55 +5446,55 @@
       <c r="R81" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="S81" s="11" t="s">
+      <c r="S81" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T81" s="11" t="s">
+      <c r="T81" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="U81" s="11" t="s">
+      <c r="U81" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="V81" s="11" t="s">
+      <c r="V81" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="W81" s="11"/>
+      <c r="W81" s="7"/>
       <c r="X81" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y81" s="11" t="s">
+      <c r="Y81" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z81" s="11" t="s">
+      <c r="Z81" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AA81" s="11" t="s">
+      <c r="AA81" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AB81" s="11" t="s">
+      <c r="AB81" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AC81" s="12">
+      <c r="AC81" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E82" s="3"/>
-      <c r="F82" s="11"/>
-      <c r="G82" s="11"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
       <c r="K82" s="6"/>
       <c r="L82" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="M82" s="11" t="s">
+      <c r="M82" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="N82" s="11" t="s">
+      <c r="N82" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="O82" s="12" t="s">
+      <c r="O82" s="8" t="s">
         <v>151</v>
       </c>
       <c r="P82" s="4" t="s">
@@ -5577,55 +5503,55 @@
       <c r="R82" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S82" s="11" t="s">
+      <c r="S82" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T82" s="11" t="s">
+      <c r="T82" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U82" s="11" t="s">
+      <c r="U82" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="V82" s="11" t="s">
+      <c r="V82" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="W82" s="11"/>
+      <c r="W82" s="7"/>
       <c r="X82" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Y82" s="11" t="s">
+      <c r="Y82" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z82" s="11" t="s">
+      <c r="Z82" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AA82" s="11" t="s">
+      <c r="AA82" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AB82" s="11" t="s">
+      <c r="AB82" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AC82" s="12">
+      <c r="AC82" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E83" s="3"/>
-      <c r="F83" s="11"/>
-      <c r="G83" s="11"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
       <c r="K83" s="6"/>
       <c r="L83" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="M83" s="13" t="s">
+      <c r="M83" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="N83" s="13" t="s">
+      <c r="N83" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="O83" s="14" t="s">
+      <c r="O83" s="4" t="s">
         <v>147</v>
       </c>
       <c r="P83" s="4" t="s">
@@ -5634,55 +5560,55 @@
       <c r="R83" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="S83" s="11" t="s">
+      <c r="S83" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T83" s="11" t="s">
+      <c r="T83" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U83" s="11" t="s">
+      <c r="U83" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="V83" s="11" t="s">
+      <c r="V83" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="W83" s="11"/>
+      <c r="W83" s="7"/>
       <c r="X83" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Y83" s="11" t="s">
+      <c r="Y83" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z83" s="11" t="s">
+      <c r="Z83" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AA83" s="11" t="s">
+      <c r="AA83" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AB83" s="11" t="s">
+      <c r="AB83" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="AC83" s="12">
+      <c r="AC83" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E84" s="3"/>
-      <c r="F84" s="11"/>
-      <c r="G84" s="11"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
       <c r="K84" s="6"/>
       <c r="L84" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="M84" s="13" t="s">
+      <c r="M84" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="N84" s="13" t="s">
+      <c r="N84" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="O84" s="14" t="s">
+      <c r="O84" s="4" t="s">
         <v>145</v>
       </c>
       <c r="P84" s="4" t="s">
@@ -5691,52 +5617,52 @@
       <c r="R84" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S84" s="11" t="s">
+      <c r="S84" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T84" s="11" t="s">
+      <c r="T84" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U84" s="11" t="s">
+      <c r="U84" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V84" s="11" t="s">
+      <c r="V84" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="W84" s="11"/>
+      <c r="W84" s="7"/>
       <c r="X84" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Y84" s="11" t="s">
+      <c r="Y84" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z84" s="11" t="s">
+      <c r="Z84" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AA84" s="11" t="s">
+      <c r="AA84" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AB84" s="11" t="s">
+      <c r="AB84" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AC84" s="12">
+      <c r="AC84" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E85" s="3"/>
-      <c r="F85" s="11"/>
-      <c r="G85" s="11"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
       <c r="K85" s="6"/>
       <c r="L85" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="M85" s="11" t="s">
+      <c r="M85" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="N85" s="11" t="s">
+      <c r="N85" s="7" t="s">
         <v>144</v>
       </c>
       <c r="O85" s="4" t="s">
@@ -5748,42 +5674,42 @@
       <c r="R85" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="S85" s="11" t="s">
+      <c r="S85" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T85" s="11" t="s">
+      <c r="T85" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U85" s="11" t="s">
+      <c r="U85" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V85" s="11" t="s">
+      <c r="V85" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="W85" s="11"/>
+      <c r="W85" s="7"/>
       <c r="X85" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y85" s="11" t="s">
+      <c r="Y85" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z85" s="11" t="s">
+      <c r="Z85" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AA85" s="11" t="s">
+      <c r="AA85" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AB85" s="11" t="s">
+      <c r="AB85" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AC85" s="12">
+      <c r="AC85" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="86" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E86" s="3"/>
-      <c r="F86" s="11"/>
-      <c r="G86" s="11"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
       <c r="K86" s="6"/>
@@ -5805,120 +5731,118 @@
       <c r="R86" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="S86" s="11" t="s">
+      <c r="S86" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T86" s="11" t="s">
+      <c r="T86" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U86" s="11" t="s">
+      <c r="U86" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V86" s="11" t="s">
+      <c r="V86" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="W86" s="11"/>
+      <c r="W86" s="7"/>
       <c r="X86" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Y86" s="11" t="s">
+      <c r="Y86" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z86" s="11" t="s">
+      <c r="Z86" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AA86" s="11" t="s">
+      <c r="AA86" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AB86" s="11" t="s">
+      <c r="AB86" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AC86" s="12">
+      <c r="AC86" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E87" s="3"/>
-      <c r="F87" s="11"/>
-      <c r="G87" s="11"/>
-      <c r="H87" s="11"/>
-      <c r="I87" s="11"/>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
+      <c r="I87" s="7"/>
       <c r="R87" s="3"/>
       <c r="S87" s="4"/>
-      <c r="T87" s="11"/>
-      <c r="U87" s="11"/>
-      <c r="V87" s="11"/>
-      <c r="W87" s="11"/>
-      <c r="X87" s="12"/>
+      <c r="T87" s="7"/>
+      <c r="U87" s="7"/>
+      <c r="V87" s="7"/>
+      <c r="W87" s="7"/>
+      <c r="X87" s="8"/>
     </row>
     <row r="88" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E88" s="3"/>
-      <c r="F88" s="11"/>
-      <c r="G88" s="11"/>
-      <c r="H88" s="11"/>
-      <c r="I88" s="11"/>
-      <c r="W88" s="11"/>
-      <c r="X88" s="12"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="7"/>
+      <c r="I88" s="7"/>
+      <c r="W88" s="7"/>
+      <c r="X88" s="8"/>
     </row>
     <row r="89" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E89" s="3"/>
-      <c r="F89" s="11"/>
-      <c r="G89" s="11"/>
-      <c r="H89" s="11"/>
-      <c r="I89" s="11"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
+      <c r="H89" s="7"/>
+      <c r="I89" s="7"/>
       <c r="L89" s="3"/>
       <c r="P89" s="4"/>
-      <c r="R89" s="15"/>
       <c r="S89" s="3"/>
-      <c r="T89" s="11"/>
-      <c r="U89" s="11"/>
-      <c r="V89" s="11"/>
-      <c r="W89" s="11"/>
-      <c r="X89" s="12"/>
+      <c r="T89" s="7"/>
+      <c r="U89" s="7"/>
+      <c r="V89" s="7"/>
+      <c r="W89" s="7"/>
+      <c r="X89" s="8"/>
     </row>
     <row r="90" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E90" s="3"/>
-      <c r="F90" s="11"/>
-      <c r="G90" s="11"/>
-      <c r="H90" s="11"/>
-      <c r="I90" s="11"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="7"/>
+      <c r="I90" s="7"/>
       <c r="L90" s="3"/>
       <c r="P90" s="4"/>
-      <c r="R90" s="15"/>
       <c r="S90" s="3"/>
-      <c r="T90" s="11"/>
-      <c r="U90" s="11"/>
-      <c r="V90" s="11"/>
-      <c r="W90" s="11"/>
-      <c r="X90" s="12"/>
+      <c r="T90" s="7"/>
+      <c r="U90" s="7"/>
+      <c r="V90" s="7"/>
+      <c r="W90" s="7"/>
+      <c r="X90" s="8"/>
     </row>
     <row r="91" spans="5:29" ht="21" x14ac:dyDescent="0.3">
       <c r="E91" s="3"/>
-      <c r="F91" s="11"/>
-      <c r="G91" s="11"/>
-      <c r="H91" s="11"/>
-      <c r="I91" s="11"/>
-      <c r="M91" s="17" t="s">
+      <c r="F91" s="7"/>
+      <c r="G91" s="7"/>
+      <c r="H91" s="7"/>
+      <c r="I91" s="7"/>
+      <c r="M91" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="N91" s="17"/>
-      <c r="O91" s="17"/>
-      <c r="P91" s="17"/>
-      <c r="Q91" s="17"/>
-      <c r="R91" s="17"/>
-      <c r="S91" s="17"/>
-      <c r="T91" s="17"/>
-      <c r="U91" s="17"/>
-      <c r="V91" s="17"/>
-      <c r="W91" s="17"/>
-      <c r="X91" s="17"/>
+      <c r="N91" s="14"/>
+      <c r="O91" s="14"/>
+      <c r="P91" s="14"/>
+      <c r="Q91" s="14"/>
+      <c r="R91" s="14"/>
+      <c r="S91" s="14"/>
+      <c r="T91" s="14"/>
+      <c r="U91" s="14"/>
+      <c r="V91" s="14"/>
+      <c r="W91" s="14"/>
+      <c r="X91" s="14"/>
     </row>
     <row r="92" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E92" s="3"/>
-      <c r="F92" s="11"/>
-      <c r="G92" s="11"/>
-      <c r="H92" s="11"/>
-      <c r="I92" s="11"/>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7"/>
+      <c r="H92" s="7"/>
+      <c r="I92" s="7"/>
       <c r="O92" s="3" t="s">
         <v>157</v>
       </c>
@@ -5928,10 +5852,10 @@
     </row>
     <row r="93" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E93" s="3"/>
-      <c r="F93" s="11"/>
-      <c r="G93" s="11"/>
-      <c r="H93" s="11"/>
-      <c r="I93" s="11"/>
+      <c r="F93" s="7"/>
+      <c r="G93" s="7"/>
+      <c r="H93" s="7"/>
+      <c r="I93" s="7"/>
       <c r="N93" s="3" t="s">
         <v>50</v>
       </c>
@@ -5962,10 +5886,10 @@
     </row>
     <row r="94" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E94" s="3"/>
-      <c r="F94" s="11"/>
-      <c r="G94" s="11"/>
-      <c r="H94" s="11"/>
-      <c r="I94" s="11"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
+      <c r="I94" s="7"/>
       <c r="L94" s="5"/>
       <c r="M94" s="3" t="s">
         <v>0</v>
@@ -5986,624 +5910,703 @@
       <c r="S94" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="T94" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="U94" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="V94" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="W94" s="11" t="s">
+      <c r="T94" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U94" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V94" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W94" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="X94" s="12">
+      <c r="X94" s="8">
         <v>-1</v>
       </c>
     </row>
     <row r="95" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E95" s="3"/>
-      <c r="F95" s="11"/>
-      <c r="G95" s="11"/>
-      <c r="H95" s="11"/>
-      <c r="I95" s="11"/>
+      <c r="F95" s="7"/>
+      <c r="G95" s="7"/>
+      <c r="H95" s="7"/>
+      <c r="I95" s="7"/>
       <c r="K95" s="3"/>
-      <c r="L95" s="11"/>
+      <c r="L95" s="7"/>
       <c r="M95" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="N95" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O95" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P95" s="11" t="s">
+      <c r="N95" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O95" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P95" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="Q95" s="11" t="s">
+      <c r="Q95" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R95" s="15"/>
       <c r="S95" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="T95" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="U95" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="V95" s="11" t="s">
+      <c r="T95" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U95" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V95" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="W95" s="11" t="s">
+      <c r="W95" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="X95" s="12">
+      <c r="X95" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="5:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E96" s="3"/>
-      <c r="F96" s="11"/>
-      <c r="G96" s="11"/>
-      <c r="H96" s="11"/>
-      <c r="I96" s="11"/>
+      <c r="F96" s="7"/>
+      <c r="G96" s="7"/>
+      <c r="H96" s="7"/>
+      <c r="I96" s="7"/>
       <c r="K96" s="3"/>
-      <c r="L96" s="11"/>
+      <c r="L96" s="7"/>
       <c r="M96" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N96" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O96" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P96" s="11" t="s">
+      <c r="N96" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O96" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P96" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Q96" s="11" t="s">
+      <c r="Q96" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R96" s="16"/>
+      <c r="R96" s="9"/>
       <c r="S96" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="T96" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="U96" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="V96" s="11" t="s">
+      <c r="T96" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U96" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V96" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="W96" s="11" t="s">
+      <c r="W96" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="X96" s="12">
+      <c r="X96" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E97" s="3"/>
-      <c r="F97" s="11"/>
-      <c r="G97" s="11"/>
-      <c r="H97" s="11"/>
-      <c r="I97" s="11"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="7"/>
+      <c r="H97" s="7"/>
+      <c r="I97" s="7"/>
       <c r="K97" s="3"/>
-      <c r="L97" s="11"/>
+      <c r="L97" s="7"/>
       <c r="M97" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N97" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O97" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P97" s="11" t="s">
+      <c r="N97" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O97" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P97" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="Q97" s="11" t="s">
+      <c r="Q97" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R97" s="16"/>
+      <c r="R97" s="9"/>
       <c r="S97" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="T97" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="U97" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="V97" s="11" t="s">
+      <c r="T97" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U97" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V97" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="W97" s="11" t="s">
+      <c r="W97" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="X97" s="12">
+      <c r="X97" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E98" s="3"/>
-      <c r="F98" s="11"/>
-      <c r="G98" s="11"/>
-      <c r="H98" s="11"/>
-      <c r="I98" s="11"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="7"/>
+      <c r="H98" s="7"/>
+      <c r="I98" s="7"/>
       <c r="M98" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N98" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O98" s="11" t="s">
+      <c r="N98" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O98" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="P98" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q98" s="11" t="s">
+      <c r="P98" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q98" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R98" s="16"/>
+      <c r="R98" s="9"/>
       <c r="S98" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="T98" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="U98" s="11" t="s">
+      <c r="T98" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U98" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V98" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="W98" s="11" t="s">
+      <c r="V98" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W98" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="X98" s="12">
+      <c r="X98" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E99" s="3"/>
-      <c r="F99" s="11"/>
-      <c r="G99" s="11"/>
-      <c r="H99" s="11"/>
-      <c r="I99" s="11"/>
+      <c r="F99" s="7"/>
+      <c r="G99" s="7"/>
+      <c r="H99" s="7"/>
+      <c r="I99" s="7"/>
       <c r="K99" s="3"/>
-      <c r="L99" s="11"/>
+      <c r="L99" s="7"/>
       <c r="M99" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N99" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O99" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P99" s="11" t="s">
+      <c r="N99" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O99" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P99" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q99" s="11" t="s">
+      <c r="Q99" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R99" s="15"/>
       <c r="S99" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T99" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="U99" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="V99" s="11" t="s">
+      <c r="T99" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U99" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V99" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="W99" s="11" t="s">
+      <c r="W99" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="X99" s="12">
+      <c r="X99" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E100" s="3"/>
-      <c r="F100" s="11"/>
-      <c r="G100" s="11"/>
-      <c r="H100" s="11"/>
-      <c r="I100" s="11"/>
+      <c r="F100" s="7"/>
+      <c r="G100" s="7"/>
+      <c r="H100" s="7"/>
+      <c r="I100" s="7"/>
       <c r="K100" s="3"/>
-      <c r="L100" s="11"/>
+      <c r="L100" s="7"/>
       <c r="M100" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N100" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O100" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P100" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q100" s="11" t="s">
+      <c r="N100" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O100" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P100" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q100" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="R100" s="15"/>
       <c r="S100" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="T100" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="U100" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="V100" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="W100" s="11" t="s">
+      <c r="T100" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U100" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V100" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W100" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="X100" s="12">
+      <c r="X100" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E101" s="3"/>
-      <c r="F101" s="11"/>
-      <c r="G101" s="11"/>
-      <c r="H101" s="11"/>
-      <c r="I101" s="11"/>
+      <c r="F101" s="7"/>
+      <c r="G101" s="7"/>
+      <c r="H101" s="7"/>
+      <c r="I101" s="7"/>
       <c r="K101" s="3"/>
-      <c r="L101" s="11"/>
+      <c r="L101" s="7"/>
       <c r="M101" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N101" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O101" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P101" s="11" t="s">
+      <c r="N101" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O101" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P101" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="Q101" s="11" t="s">
+      <c r="Q101" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="R101" s="15"/>
       <c r="S101" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="T101" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="U101" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="V101" s="11" t="s">
+      <c r="T101" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U101" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V101" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="W101" s="11" t="s">
+      <c r="W101" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="X101" s="12">
+      <c r="X101" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E102" s="3"/>
-      <c r="F102" s="11"/>
-      <c r="G102" s="11"/>
-      <c r="H102" s="11"/>
-      <c r="I102" s="11"/>
+      <c r="F102" s="7"/>
+      <c r="G102" s="7"/>
+      <c r="H102" s="7"/>
+      <c r="I102" s="7"/>
       <c r="K102" s="3"/>
-      <c r="L102" s="11"/>
+      <c r="L102" s="7"/>
       <c r="M102" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N102" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O102" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P102" s="11" t="s">
+      <c r="N102" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O102" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P102" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="Q102" s="11" t="s">
+      <c r="Q102" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="R102" s="15"/>
       <c r="S102" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="T102" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="U102" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="V102" s="11" t="s">
+      <c r="T102" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U102" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V102" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="W102" s="11" t="s">
+      <c r="W102" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="X102" s="12">
+      <c r="X102" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E103" s="3"/>
-      <c r="F103" s="11"/>
-      <c r="G103" s="11"/>
-      <c r="H103" s="11"/>
-      <c r="I103" s="11"/>
+      <c r="F103" s="7"/>
+      <c r="G103" s="7"/>
+      <c r="H103" s="7"/>
+      <c r="I103" s="7"/>
       <c r="L103" s="6"/>
       <c r="M103" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N103" s="11" t="s">
+      <c r="N103" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="O103" s="11" t="s">
+      <c r="O103" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="P103" s="11" t="s">
+      <c r="P103" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="Q103" s="11" t="s">
+      <c r="Q103" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="R103" s="15"/>
       <c r="S103" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="T103" s="11" t="s">
+      <c r="T103" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="U103" s="11" t="s">
+      <c r="U103" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="V103" s="11" t="s">
+      <c r="V103" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W103" s="11" t="s">
+      <c r="W103" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="X103" s="12">
+      <c r="X103" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="104" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E104" s="3"/>
-      <c r="F104" s="11"/>
-      <c r="G104" s="11"/>
-      <c r="H104" s="11"/>
-      <c r="I104" s="11"/>
+      <c r="F104" s="7"/>
+      <c r="G104" s="7"/>
+      <c r="H104" s="7"/>
+      <c r="I104" s="7"/>
       <c r="L104" s="3"/>
       <c r="M104" s="4"/>
       <c r="N104" s="4"/>
       <c r="O104" s="4"/>
       <c r="P104" s="4"/>
-      <c r="R104" s="15"/>
       <c r="S104" s="3"/>
-      <c r="T104" s="11"/>
-      <c r="U104" s="11"/>
-      <c r="V104" s="11"/>
-      <c r="W104" s="11"/>
-      <c r="X104" s="12"/>
+      <c r="T104" s="7"/>
+      <c r="U104" s="7"/>
+      <c r="V104" s="7"/>
+      <c r="W104" s="7"/>
+      <c r="X104" s="8"/>
     </row>
     <row r="105" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E105" s="3"/>
-      <c r="F105" s="11"/>
-      <c r="G105" s="11"/>
-      <c r="H105" s="11"/>
-      <c r="I105" s="11"/>
+      <c r="F105" s="7"/>
+      <c r="G105" s="7"/>
+      <c r="H105" s="7"/>
+      <c r="I105" s="7"/>
       <c r="L105" s="3"/>
       <c r="M105" s="4"/>
       <c r="N105" s="4"/>
       <c r="O105" s="4"/>
       <c r="P105" s="4"/>
-      <c r="R105" s="15"/>
       <c r="S105" s="3"/>
-      <c r="T105" s="11"/>
-      <c r="U105" s="11"/>
-      <c r="V105" s="11"/>
-      <c r="W105" s="11"/>
-      <c r="X105" s="12"/>
+      <c r="T105" s="7"/>
+      <c r="U105" s="7"/>
+      <c r="V105" s="7"/>
+      <c r="W105" s="7"/>
+      <c r="X105" s="8"/>
     </row>
     <row r="106" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E106" s="3"/>
-      <c r="F106" s="11"/>
-      <c r="G106" s="11"/>
-      <c r="H106" s="11"/>
-      <c r="I106" s="11"/>
+      <c r="F106" s="7"/>
+      <c r="G106" s="7"/>
+      <c r="H106" s="7"/>
+      <c r="I106" s="7"/>
       <c r="L106" s="3"/>
       <c r="M106" s="4"/>
       <c r="N106" s="4"/>
       <c r="O106" s="4"/>
       <c r="P106" s="4"/>
-      <c r="R106" s="16"/>
+      <c r="R106" s="9"/>
       <c r="S106" s="3"/>
-      <c r="T106" s="11"/>
-      <c r="U106" s="11"/>
-      <c r="V106" s="11"/>
-      <c r="W106" s="11"/>
-      <c r="X106" s="12"/>
+      <c r="T106" s="7"/>
+      <c r="U106" s="7"/>
+      <c r="V106" s="7"/>
+      <c r="W106" s="7"/>
+      <c r="X106" s="8"/>
     </row>
     <row r="107" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E107" s="3"/>
-      <c r="F107" s="11"/>
-      <c r="G107" s="11"/>
-      <c r="H107" s="11"/>
-      <c r="I107" s="11"/>
+      <c r="F107" s="7"/>
+      <c r="G107" s="7"/>
+      <c r="H107" s="7"/>
+      <c r="I107" s="7"/>
       <c r="L107" s="3"/>
       <c r="M107" s="4"/>
       <c r="N107" s="4"/>
       <c r="O107" s="4"/>
       <c r="P107" s="4"/>
-      <c r="R107" s="16"/>
+      <c r="R107" s="9"/>
       <c r="S107" s="3"/>
-      <c r="T107" s="11"/>
-      <c r="U107" s="11"/>
-      <c r="V107" s="11"/>
-      <c r="W107" s="11"/>
-      <c r="X107" s="12"/>
+      <c r="T107" s="7"/>
+      <c r="U107" s="7"/>
+      <c r="V107" s="7"/>
+      <c r="W107" s="7"/>
+      <c r="X107" s="8"/>
     </row>
     <row r="108" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E108" s="3"/>
-      <c r="F108" s="11"/>
-      <c r="G108" s="11"/>
-      <c r="H108" s="11"/>
-      <c r="I108" s="11"/>
+      <c r="F108" s="7"/>
+      <c r="G108" s="7"/>
+      <c r="H108" s="7"/>
+      <c r="I108" s="7"/>
       <c r="L108" s="3"/>
       <c r="M108" s="4"/>
       <c r="N108" s="4"/>
       <c r="O108" s="4"/>
       <c r="P108" s="4"/>
-      <c r="R108" s="16"/>
+      <c r="R108" s="9"/>
       <c r="S108" s="3"/>
-      <c r="T108" s="11"/>
-      <c r="U108" s="11"/>
-      <c r="V108" s="11"/>
-      <c r="W108" s="11"/>
-      <c r="X108" s="12"/>
+      <c r="T108" s="7"/>
+      <c r="U108" s="7"/>
+      <c r="V108" s="7"/>
+      <c r="W108" s="7"/>
+      <c r="X108" s="8"/>
     </row>
     <row r="109" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E109" s="3"/>
-      <c r="F109" s="11"/>
-      <c r="G109" s="11"/>
-      <c r="H109" s="11"/>
-      <c r="I109" s="11"/>
+      <c r="F109" s="7"/>
+      <c r="G109" s="7"/>
+      <c r="H109" s="7"/>
+      <c r="I109" s="7"/>
       <c r="L109" s="3"/>
       <c r="M109" s="4"/>
       <c r="N109" s="4"/>
       <c r="O109" s="4"/>
       <c r="P109" s="4"/>
-      <c r="R109" s="16"/>
+      <c r="R109" s="9"/>
       <c r="S109" s="3"/>
-      <c r="T109" s="11"/>
-      <c r="U109" s="11"/>
-      <c r="V109" s="11"/>
-      <c r="W109" s="11"/>
-      <c r="X109" s="12"/>
+      <c r="T109" s="7"/>
+      <c r="U109" s="7"/>
+      <c r="V109" s="7"/>
+      <c r="W109" s="7"/>
+      <c r="X109" s="8"/>
     </row>
     <row r="110" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E110" s="3"/>
-      <c r="F110" s="11"/>
-      <c r="G110" s="11"/>
-      <c r="H110" s="11"/>
-      <c r="I110" s="11"/>
+      <c r="F110" s="7"/>
+      <c r="G110" s="7"/>
+      <c r="H110" s="7"/>
+      <c r="I110" s="7"/>
       <c r="L110" s="3"/>
       <c r="M110" s="4"/>
       <c r="N110" s="4"/>
       <c r="O110" s="4"/>
       <c r="P110" s="4"/>
-      <c r="R110" s="16"/>
+      <c r="R110" s="9"/>
       <c r="S110" s="3"/>
-      <c r="T110" s="11"/>
-      <c r="U110" s="11"/>
-      <c r="V110" s="11"/>
-      <c r="W110" s="11"/>
-      <c r="X110" s="12"/>
-    </row>
-    <row r="111" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="T110" s="7"/>
+      <c r="U110" s="7"/>
+      <c r="V110" s="7"/>
+      <c r="W110" s="7"/>
+      <c r="X110" s="8"/>
+    </row>
+    <row r="111" spans="5:24" ht="21" x14ac:dyDescent="0.3">
       <c r="E111" s="3"/>
-      <c r="F111" s="11"/>
-      <c r="G111" s="11"/>
-      <c r="H111" s="11"/>
-      <c r="I111" s="11"/>
+      <c r="F111" s="7"/>
+      <c r="G111" s="7"/>
+      <c r="H111" s="7"/>
+      <c r="I111" s="7"/>
       <c r="L111" s="3"/>
-      <c r="M111" s="4"/>
-      <c r="N111" s="4"/>
-      <c r="O111" s="4"/>
-      <c r="P111" s="4"/>
-      <c r="R111" s="16"/>
-      <c r="S111" s="3"/>
-      <c r="T111" s="11"/>
-      <c r="U111" s="11"/>
-      <c r="V111" s="11"/>
-      <c r="W111" s="11"/>
-      <c r="X111" s="12"/>
+      <c r="M111" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="N111" s="14"/>
+      <c r="O111" s="14"/>
+      <c r="P111" s="14"/>
+      <c r="Q111" s="14"/>
+      <c r="R111" s="14"/>
+      <c r="S111" s="14"/>
+      <c r="T111" s="14"/>
+      <c r="U111" s="14"/>
+      <c r="V111" s="14"/>
+      <c r="W111" s="14"/>
+      <c r="X111" s="14"/>
     </row>
     <row r="112" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E112" s="3"/>
-      <c r="F112" s="11"/>
-      <c r="G112" s="11"/>
-      <c r="H112" s="11"/>
-      <c r="I112" s="11"/>
+      <c r="F112" s="7"/>
+      <c r="G112" s="7"/>
+      <c r="H112" s="7"/>
+      <c r="I112" s="7"/>
       <c r="L112" s="3"/>
-      <c r="M112" s="4"/>
-      <c r="N112" s="4"/>
-      <c r="O112" s="4"/>
-      <c r="P112" s="4"/>
-      <c r="R112" s="16"/>
+      <c r="N112" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O112" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="P112" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q112" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="R112" s="9"/>
       <c r="S112" s="3"/>
-      <c r="T112" s="11"/>
-      <c r="U112" s="11"/>
-      <c r="V112" s="11"/>
-      <c r="W112" s="11"/>
-      <c r="X112" s="12"/>
+      <c r="T112" s="7"/>
+      <c r="U112" s="7"/>
+      <c r="V112" s="7"/>
+      <c r="W112" s="7"/>
+      <c r="X112" s="8"/>
     </row>
     <row r="113" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E113" s="3"/>
-      <c r="F113" s="11"/>
-      <c r="G113" s="11"/>
-      <c r="H113" s="11"/>
-      <c r="I113" s="11"/>
+      <c r="F113" s="7"/>
+      <c r="G113" s="7"/>
+      <c r="H113" s="7"/>
+      <c r="I113" s="7"/>
       <c r="L113" s="3"/>
-      <c r="M113" s="4"/>
-      <c r="N113" s="4"/>
-      <c r="O113" s="4"/>
-      <c r="P113" s="4"/>
-      <c r="R113" s="16"/>
+      <c r="M113" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N113" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O113" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P113" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q113" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R113" s="9"/>
       <c r="S113" s="3"/>
-      <c r="T113" s="11"/>
-      <c r="U113" s="11"/>
-      <c r="V113" s="11"/>
-      <c r="W113" s="11"/>
-      <c r="X113" s="12"/>
+      <c r="T113" s="7"/>
+      <c r="U113" s="7"/>
+      <c r="V113" s="7"/>
+      <c r="W113" s="7"/>
+      <c r="X113" s="8"/>
     </row>
     <row r="114" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E114" s="3"/>
-      <c r="F114" s="11"/>
-      <c r="G114" s="11"/>
-      <c r="H114" s="11"/>
-      <c r="I114" s="11"/>
+      <c r="F114" s="7"/>
+      <c r="G114" s="7"/>
+      <c r="H114" s="7"/>
+      <c r="I114" s="7"/>
+      <c r="M114" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N114" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O114" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P114" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q114" s="7" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="115" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E115" s="3"/>
-      <c r="F115" s="11"/>
-      <c r="G115" s="11"/>
-      <c r="H115" s="11"/>
-      <c r="I115" s="11"/>
+      <c r="F115" s="7"/>
+      <c r="G115" s="7"/>
+      <c r="H115" s="7"/>
+      <c r="I115" s="7"/>
+      <c r="M115" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N115" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="O115" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P115" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q115" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M116" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N116" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="O116" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P116" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q116" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="5:24" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M117" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N117" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O117" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P117" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q117" s="7" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AA72:AA80">
     <sortCondition ref="AA72:AA80"/>
   </sortState>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="M111:X111"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="S2:X2"/>
+    <mergeCell ref="L1:X1"/>
     <mergeCell ref="M91:X91"/>
     <mergeCell ref="L60:P60"/>
     <mergeCell ref="R60:V60"/>
     <mergeCell ref="X60:AC60"/>
     <mergeCell ref="L59:AC59"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="S2:X2"/>
-    <mergeCell ref="L1:X1"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>